<commit_message>
Minor adjustment to civic_number and 1 insert statement.
</commit_message>
<xml_diff>
--- a/04_02327Effort_2024.xlsx
+++ b/04_02327Effort_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SWT\02327 - Database 24F\Mandatory group assignment\DB24-G4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58C7967-2F92-4366-B3B1-81BF264C2D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F332A1-0A8B-4C3E-A612-DFE1C720ABDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="240" windowWidth="28800" windowHeight="15240" xr2:uid="{92146609-C4DC-4D5F-9EE3-E7911B4BB962}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{92146609-C4DC-4D5F-9EE3-E7911B4BB962}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Member</t>
   </si>
@@ -83,20 +83,35 @@
     <t>7. SQL Programming</t>
   </si>
   <si>
-    <t>AVERAGE</t>
+    <t>Adrian Macauley s225733</t>
+  </si>
+  <si>
+    <t>Peter Juul s215781</t>
+  </si>
+  <si>
+    <t>Sivalaxmanan B. Krishnapillai s245231</t>
+  </si>
+  <si>
+    <t>AVERAGE in percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -119,8 +134,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,16 +473,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9D042F-5A87-40EE-8C5C-7E326AB8B5BE}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="3" max="10" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="9" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -522,7 +542,61 @@
         <v>8</v>
       </c>
       <c r="J2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>15</v>
+      </c>
+      <c r="C3">
+        <v>33</v>
+      </c>
+      <c r="D3">
+        <v>33</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="J3">
+        <f>AVERAGE(C3:I3)</f>
+        <v>38.666666666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <v>33</v>
+      </c>
+      <c r="E4">
+        <v>23</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J5" si="0">AVERAGE(C4:I4)</f>
+        <v>29.666666666666668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>33</v>
+      </c>
+      <c r="E5">
+        <v>45</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>